<commit_message>
Add values of 1st list
</commit_message>
<xml_diff>
--- a/Test/Kursach.xlsx
+++ b/Test/Kursach.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Общая информация" sheetId="3" r:id="rId1"/>
     <sheet name="Варианты" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -165,13 +165,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -181,6 +178,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -488,7 +487,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +505,7 @@
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="8">
         <v>20</v>
       </c>
     </row>
@@ -514,7 +513,7 @@
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="8">
         <v>5</v>
       </c>
     </row>
@@ -522,7 +521,7 @@
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="8">
         <v>100</v>
       </c>
     </row>
@@ -530,15 +529,15 @@
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="8">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="8">
         <v>0.14000000000000001</v>
       </c>
     </row>
@@ -546,23 +545,23 @@
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="8">
         <v>0.11</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="8">
         <v>0.2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="8">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
@@ -590,20 +589,20 @@
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="8">
         <f>0.7</f>
         <v>0.7</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="8">
         <v>0.9</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="8">
         <v>1</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="8">
         <v>1</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="8">
         <v>0.8</v>
       </c>
     </row>
@@ -611,19 +610,19 @@
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="9">
         <v>15</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="8">
         <v>10</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="8">
         <v>6</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="8">
         <v>3</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="8">
         <v>2</v>
       </c>
     </row>
@@ -631,161 +630,161 @@
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="8">
         <v>0.2</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="8">
         <v>0.4</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="8">
         <v>0.4</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -807,109 +806,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="9">
+      <c r="B2" s="6">
         <v>1</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="6">
         <v>2</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="6">
         <v>3</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="6">
         <v>4</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="6">
         <v>5</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="6">
         <v>6</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="6">
         <v>7</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="6">
         <v>8</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="6">
         <v>9</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="6">
         <v>10</v>
       </c>
-      <c r="L2" s="9">
+      <c r="L2" s="6">
         <v>11</v>
       </c>
-      <c r="M2" s="9">
+      <c r="M2" s="6">
         <v>12</v>
       </c>
-      <c r="N2" s="9">
+      <c r="N2" s="6">
         <v>13</v>
       </c>
-      <c r="O2" s="9">
+      <c r="O2" s="6">
         <v>14</v>
       </c>
-      <c r="P2" s="9">
+      <c r="P2" s="6">
         <v>15</v>
       </c>
-      <c r="Q2" s="9">
+      <c r="Q2" s="6">
         <v>16</v>
       </c>
-      <c r="R2" s="9">
+      <c r="R2" s="6">
         <v>17</v>
       </c>
-      <c r="S2" s="9">
+      <c r="S2" s="6">
         <v>18</v>
       </c>
-      <c r="T2" s="9">
+      <c r="T2" s="6">
         <v>19</v>
       </c>
-      <c r="U2" s="9">
+      <c r="U2" s="6">
         <v>20</v>
       </c>
-      <c r="V2" s="9">
+      <c r="V2" s="6">
         <v>21</v>
       </c>
-      <c r="W2" s="9">
+      <c r="W2" s="6">
         <v>22</v>
       </c>
-      <c r="X2" s="9">
+      <c r="X2" s="6">
         <v>23</v>
       </c>
-      <c r="Y2" s="9">
+      <c r="Y2" s="6">
         <v>24</v>
       </c>
-      <c r="Z2" s="9">
+      <c r="Z2" s="6">
         <v>25</v>
       </c>
     </row>

</xml_diff>